<commit_message>
For PCBWAY March 03
</commit_message>
<xml_diff>
--- a/ESC_dev_board/BOM/Bill of Materials-ESC_dev_board.xlsx
+++ b/ESC_dev_board/BOM/Bill of Materials-ESC_dev_board.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Poorna\OneDrive - University of Victoria\University\Clubs\AUVic\Hardware\ESC_dev_board\ESC_dev_board\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Poorna\OneDrive - University of Victoria\University\Clubs\AUVic\Hardware\PCB-ESC-Dev-Board\ESC_dev_board\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E89A26EC-0F9A-4681-98DB-35AB59608984}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{521CA1DB-B42F-402D-A21C-36A68E0DEDF0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6816" yWindow="1140" windowWidth="13824" windowHeight="7176" xr2:uid="{7AA85207-FF5B-4427-B362-4316CC6FEFD9}"/>
+    <workbookView xWindow="6816" yWindow="1140" windowWidth="13824" windowHeight="7176" xr2:uid="{5175610F-6DF1-41A9-8846-875CE28139F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-ESC_dev_board" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="77">
   <si>
     <t>Line #</t>
   </si>
@@ -78,6 +78,9 @@
     <t>Supplier Subtotal 1</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>1μF</t>
   </si>
   <si>
@@ -123,9 +126,6 @@
     <t>445-5098-1-ND</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>100µF</t>
   </si>
   <si>
@@ -139,9 +139,6 @@
   </si>
   <si>
     <t>875115652007</t>
-  </si>
-  <si>
-    <t>Unknown</t>
   </si>
   <si>
     <t>732-11942-1-ND</t>
@@ -330,10 +327,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -649,7 +646,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA7EEE8C-DC64-46D8-8A19-E2322CB2D65C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB302E4C-2966-4BE7-9C7A-9172F4972530}">
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -716,436 +713,448 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="A2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="3">
+      <c r="E2" s="4"/>
+      <c r="F2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="4">
         <v>1</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="3">
+      <c r="L2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="4">
         <v>0.17</v>
       </c>
-      <c r="N2" s="3">
+      <c r="N2" s="4">
         <v>0.17</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="72" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="3">
+      <c r="D3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="4">
         <v>1</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" s="4" t="s">
+      <c r="I3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
+      <c r="K3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
     </row>
     <row r="4" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="3">
+      <c r="E4" s="4"/>
+      <c r="F4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="4">
         <v>4</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="K4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="M4" s="3">
+      <c r="M4" s="4">
         <v>2.76</v>
       </c>
-      <c r="N4" s="3">
+      <c r="N4" s="4">
         <v>11.04</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4"/>
+      <c r="F5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="4">
+        <v>2</v>
+      </c>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="3">
-        <v>2</v>
-      </c>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
     </row>
     <row r="6" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4"/>
+      <c r="F6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="3">
-        <v>1</v>
-      </c>
-      <c r="H6" s="4" t="s">
+      <c r="I6" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="J6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="J6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="M6" s="3">
+      <c r="M6" s="4">
         <v>0.6</v>
       </c>
-      <c r="N6" s="3">
+      <c r="N6" s="4">
         <v>0.6</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4"/>
+      <c r="F7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="4">
+        <v>1</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="3">
-        <v>1</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="I7" s="4" t="s">
+      <c r="J7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="M7" s="3">
+      <c r="M7" s="4">
         <v>0.49</v>
       </c>
-      <c r="N7" s="3">
+      <c r="N7" s="4">
         <v>0.49</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="4" t="s">
+      <c r="A8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="4"/>
+      <c r="F8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="4">
+        <v>3</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="3">
-        <v>3</v>
-      </c>
-      <c r="H8" s="4" t="s">
+      <c r="I8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L8" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="I8" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="M8" s="3">
+      <c r="M8" s="4">
         <v>1.1000000000000001</v>
       </c>
-      <c r="N8" s="3">
+      <c r="N8" s="4">
         <v>3.3</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="4" t="s">
+      <c r="A9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="4"/>
+      <c r="F9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="4">
+        <v>3</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="3">
-        <v>3</v>
-      </c>
-      <c r="H9" s="4" t="s">
+      <c r="I9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="I9" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="M9" s="3">
+      <c r="M9" s="4">
         <v>1.1599999999999999</v>
       </c>
-      <c r="N9" s="3">
+      <c r="N9" s="4">
         <v>3.48</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="4" t="s">
+      <c r="A10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="4"/>
+      <c r="F10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="4">
+        <v>6</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="3">
-        <v>6</v>
-      </c>
-      <c r="H10" s="4" t="s">
+      <c r="I10" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="J10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L10" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="J10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="L10" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="M10" s="3">
+      <c r="M10" s="4">
         <v>1.9E-2</v>
       </c>
-      <c r="N10" s="3">
+      <c r="N10" s="4">
         <v>0.19</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4" t="s">
+      <c r="A11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="4"/>
+      <c r="F11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="4">
+        <v>1</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" s="3">
-        <v>1</v>
-      </c>
-      <c r="H11" s="4" t="s">
+      <c r="I11" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="J11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L11" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="J11" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="M11" s="3">
+      <c r="M11" s="4">
         <v>0.69</v>
       </c>
-      <c r="N11" s="3">
+      <c r="N11" s="4">
         <v>0.69</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4" t="s">
+      <c r="A12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="E12" s="4"/>
+      <c r="F12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="4">
+        <v>1</v>
+      </c>
+      <c r="H12" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="3">
-        <v>1</v>
-      </c>
-      <c r="H12" s="4" t="s">
+      <c r="I12" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="J12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L12" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="J12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="M12" s="3">
+      <c r="M12" s="4">
         <v>2.78</v>
       </c>
-      <c r="N12" s="3">
+      <c r="N12" s="4">
         <v>2.78</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed mistakes in BOM
</commit_message>
<xml_diff>
--- a/ESC_dev_board/BOM/Bill of Materials-ESC_dev_board.xlsx
+++ b/ESC_dev_board/BOM/Bill of Materials-ESC_dev_board.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Poorna\OneDrive - University of Victoria\University\Clubs\AUVic\Hardware\PCB-ESC-Dev-Board\ESC_dev_board\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uvicca0-my.sharepoint.com/personal/poornack_uvic_ca/Documents/University/Clubs/AUVic/Hardware/PCB-ESC-Dev-Board/ESC_dev_board/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{521CA1DB-B42F-402D-A21C-36A68E0DEDF0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BCB2EB7F-2435-4B3C-9ED2-03D65190BBEA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6816" yWindow="1140" windowWidth="13824" windowHeight="7176" xr2:uid="{5175610F-6DF1-41A9-8846-875CE28139F8}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{BF9C5145-4E05-4344-A7B3-9D04D35D7E4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-ESC_dev_board" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="81">
   <si>
     <t>Line #</t>
   </si>
@@ -105,13 +105,13 @@
     <t>Digi-Key</t>
   </si>
   <si>
-    <t>1276-1860-6-ND</t>
+    <t>1276-1860-1-ND</t>
   </si>
   <si>
     <t>0.1uF, 50V, 10%, X7R, 0603</t>
   </si>
   <si>
-    <t>0.1µF ±20% Ceramic Capacitor X7R 0603 (1608 Metric)</t>
+    <t>0.1µF ±10% Ceramic Capacitor X7R 0603 (1608 Metric)</t>
   </si>
   <si>
     <t>C6</t>
@@ -120,10 +120,13 @@
     <t>TDK</t>
   </si>
   <si>
-    <t>C1608X7R1H104M080AA</t>
-  </si>
-  <si>
-    <t>445-5098-1-ND</t>
+    <t>C1608X7R1H104K</t>
+  </si>
+  <si>
+    <t>Not Recommended for New Design</t>
+  </si>
+  <si>
+    <t>445-1314-1-ND</t>
   </si>
   <si>
     <t>100µF</t>
@@ -141,6 +144,9 @@
     <t>875115652007</t>
   </si>
   <si>
+    <t>Unknown</t>
+  </si>
+  <si>
     <t>732-11942-1-ND</t>
   </si>
   <si>
@@ -153,7 +159,13 @@
     <t>CN3, CN4</t>
   </si>
   <si>
-    <t>Digikey</t>
+    <t>Harwin</t>
+  </si>
+  <si>
+    <t>M20-9990446</t>
+  </si>
+  <si>
+    <t>952-2266-ND</t>
   </si>
   <si>
     <t>3x1, Terminal Block, Pitch: 5mm, Screw, THT</t>
@@ -646,14 +658,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB302E4C-2966-4BE7-9C7A-9172F4972530}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA4B0EBF-DCF4-4F71-B523-5F57165F1AB5}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.77734375" customWidth="1"/>
     <col min="3" max="3" width="23.88671875" customWidth="1"/>
     <col min="4" max="4" width="21.88671875" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" customWidth="1"/>
@@ -754,10 +769,8 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="72" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>14</v>
-      </c>
+    <row r="3" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="4"/>
       <c r="B3" s="3" t="s">
         <v>24</v>
       </c>
@@ -781,29 +794,33 @@
         <v>28</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="M3" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="N3" s="4">
+        <v>0.12</v>
+      </c>
     </row>
     <row r="4" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="3" t="s">
@@ -813,19 +830,19 @@
         <v>4</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="M4" s="4">
         <v>2.76</v>
@@ -839,13 +856,13 @@
         <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="3" t="s">
@@ -854,28 +871,40 @@
       <c r="G5" s="4">
         <v>2</v>
       </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
+      <c r="H5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="K5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
+        <v>22</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="M5" s="4">
+        <v>0.19</v>
+      </c>
+      <c r="N5" s="4">
+        <v>0.38</v>
+      </c>
     </row>
-    <row r="6" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="3" t="s">
@@ -885,10 +914,10 @@
         <v>1</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>21</v>
@@ -897,7 +926,7 @@
         <v>22</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="M6" s="4">
         <v>0.6</v>
@@ -906,18 +935,18 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="3" t="s">
@@ -927,10 +956,10 @@
         <v>1</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>21</v>
@@ -939,7 +968,7 @@
         <v>22</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="M7" s="4">
         <v>0.49</v>
@@ -953,13 +982,13 @@
         <v>14</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="3" t="s">
@@ -969,10 +998,10 @@
         <v>3</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>21</v>
@@ -981,13 +1010,13 @@
         <v>22</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="M8" s="4">
-        <v>1.1000000000000001</v>
+        <v>1.07</v>
       </c>
       <c r="N8" s="4">
-        <v>3.3</v>
+        <v>3.21</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
@@ -995,13 +1024,13 @@
         <v>14</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="3" t="s">
@@ -1011,10 +1040,10 @@
         <v>3</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>21</v>
@@ -1023,13 +1052,13 @@
         <v>22</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="M9" s="4">
-        <v>1.1599999999999999</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="N9" s="4">
-        <v>3.48</v>
+        <v>3.36</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
@@ -1037,13 +1066,13 @@
         <v>14</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="3" t="s">
@@ -1053,10 +1082,10 @@
         <v>6</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>21</v>
@@ -1065,7 +1094,7 @@
         <v>22</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="M10" s="4">
         <v>1.9E-2</v>
@@ -1079,13 +1108,13 @@
         <v>14</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="3" t="s">
@@ -1095,19 +1124,19 @@
         <v>1</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>22</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="M11" s="4">
         <v>0.69</v>
@@ -1121,13 +1150,13 @@
         <v>14</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="3" t="s">
@@ -1137,10 +1166,10 @@
         <v>1</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>21</v>
@@ -1149,17 +1178,322 @@
         <v>22</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="M12" s="4">
-        <v>2.78</v>
+        <v>2.7</v>
       </c>
       <c r="N12" s="4">
-        <v>2.78</v>
+        <v>2.7</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
+  <pageSetup paperSize="9" scale="55" orientation="landscape" blackAndWhite="1" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010024846BE2D35DE54A9BE8BBA42D0700AD" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="641b7ec275f27219802da9e743dd1056">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="5c534bb1-62b0-46e0-9ae3-b9112d146ccd" xmlns:ns4="8966a34b-ec6c-46f3-826c-d8f2f7d74935" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d1271ae291c08be0062a66eeb80c51a0" ns1:_="" ns3:_="" ns4:_="">
+    <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
+    <xsd:import namespace="5c534bb1-62b0-46e0-9ae3-b9112d146ccd"/>
+    <xsd:import namespace="8966a34b-ec6c-46f3-826c-d8f2f7d74935"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns3:SharingHintHash" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyProperties" minOccurs="0"/>
+                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyUIAction" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceKeyPoints" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="http://schemas.microsoft.com/sharepoint/v3" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="15" nillable="true" ma:displayName="Unified Compliance Policy Properties" ma:description="" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="16" nillable="true" ma:displayName="Unified Compliance Policy UI Action" ma:description="" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="5c534bb1-62b0-46e0-9ae3-b9112d146ccd" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="8" nillable="true" ma:displayName="Shared With" ma:description="" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="9" nillable="true" ma:displayName="Shared With Details" ma:description="" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SharingHintHash" ma:index="10" nillable="true" ma:displayName="Sharing Hint Hash" ma:description="" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="8966a34b-ec6c-46f3-826c-d8f2f7d74935" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="11" nillable="true" ma:displayName="MediaServiceMetadata" ma:description="" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="12" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:description="" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="13" nillable="true" ma:displayName="MediaServiceDateTaken" ma:description="" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="14" nillable="true" ma:displayName="MediaServiceAutoTags" ma:description="" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="17" nillable="true" ma:displayName="MediaServiceOCR" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="18" nillable="true" ma:displayName="MediaServiceLocation" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="19" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="20" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="21" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="22" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E097207D-EEA7-4831-A617-EC3845D23D22}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="5c534bb1-62b0-46e0-9ae3-b9112d146ccd"/>
+    <ds:schemaRef ds:uri="8966a34b-ec6c-46f3-826c-d8f2f7d74935"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26EB4E44-3BAD-4887-A0A9-21BEC0F9CE2A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{443AA9D1-4386-41FA-8917-3E2E668729F1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="8966a34b-ec6c-46f3-826c-d8f2f7d74935"/>
+    <ds:schemaRef ds:uri="5c534bb1-62b0-46e0-9ae3-b9112d146ccd"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>